<commit_message>
fead: added alphabetical sorting in populating the excel file
</commit_message>
<xml_diff>
--- a/170_project/attendance.xlsx
+++ b/170_project/attendance.xlsx
@@ -441,7 +441,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>roche</t>
+          <t>cyrus</t>
         </is>
       </c>
     </row>
@@ -458,24 +458,14 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>20:39:53</t>
+          <t>21:09:27</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>cyrus</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>PRESENT</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>20:30:59</t>
+          <t>roche</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: added absent feature in excel
</commit_message>
<xml_diff>
--- a/170_project/attendance.xlsx
+++ b/170_project/attendance.xlsx
@@ -429,7 +429,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>2024-12-13</t>
+          <t>2024-12-14</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -444,6 +444,16 @@
           <t>cyrus</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>PRESENT</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>14:52:41</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -458,7 +468,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>21:09:27</t>
+          <t>14:53:00</t>
         </is>
       </c>
     </row>
@@ -466,6 +476,16 @@
       <c r="A4" t="inlineStr">
         <is>
           <t>roche</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>PRESENT</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>14:52:42</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore: renamed main file and added known faces
</commit_message>
<xml_diff>
--- a/170_project/attendance.xlsx
+++ b/170_project/attendance.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,24 +441,19 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>cyrus</t>
+          <t>Barrack Obama</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>PRESENT</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>14:52:41</t>
+          <t>ABSENT</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>kiefer</t>
+          <t>Cyrus Gello Par</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -468,24 +463,53 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>14:53:00</t>
+          <t>16:46:57</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>roche</t>
+          <t>Elon Musk</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>ABSENT</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Kiefer Tayawa</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>PRESENT</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>14:52:42</t>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>16:46:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Roche Quejada</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>PRESENT</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>16:46:50</t>
         </is>
       </c>
     </row>

</xml_diff>